<commit_message>
fix issn mappings in spreadsheet
</commit_message>
<xml_diff>
--- a/marc/MARC_subfields_not_mapped.xlsx
+++ b/marc/MARC_subfields_not_mapped.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="571">
   <si>
     <t>Omission type</t>
   </si>
@@ -1740,6 +1740,15 @@
   </si>
   <si>
     <t>UNC has no data in this subfield. Consider mapping to genre_headings and subject_genre if ever meaningfully populated</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -1789,7 +1798,7 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="164" formatCode="000"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1801,7 +1810,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="000"/>
@@ -1832,12 +1841,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F2" totalsRowShown="0">
-  <autoFilter ref="A1:F2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F5" totalsRowShown="0">
+  <autoFilter ref="A1:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="MARC tag" dataDxfId="5"/>
-    <tableColumn id="6" name="Subfield" dataDxfId="0"/>
-    <tableColumn id="5" name="Field name" dataDxfId="4">
+    <tableColumn id="6" name="Subfield" dataDxfId="4"/>
+    <tableColumn id="5" name="Field name" dataDxfId="3">
       <calculatedColumnFormula>VLOOKUP(TEXT(A2, "000"),tag_lookup[],2,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Omission type"/>
@@ -1852,9 +1861,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tag_lookup" displayName="tag_lookup" ref="A1:C281" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C281"/>
   <tableColumns count="3">
-    <tableColumn id="22" uniqueName="22" name="MARC tag padded" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="23" uniqueName="23" name="Field name" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="24" uniqueName="24" name="Other note" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="22" uniqueName="22" name="MARC tag padded" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="23" uniqueName="23" name="Field name" queryTableFieldId="2" dataDxfId="1"/>
+    <tableColumn id="24" uniqueName="24" name="Other note" queryTableFieldId="3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2123,10 +2132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,6 +2184,42 @@
       </c>
       <c r="F2" t="s">
         <v>567</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>VLOOKUP(TEXT(A3, "000"),tag_lookup[],2,0)</f>
+        <v>International Standard Serial Number</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>VLOOKUP(TEXT(A4, "000"),tag_lookup[],2,0)</f>
+        <v>International Standard Serial Number</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f>VLOOKUP(TEXT(A5, "000"),tag_lookup[],2,0)</f>
+        <v>International Standard Serial Number</v>
       </c>
     </row>
   </sheetData>

</xml_diff>